<commit_message>
Add comprehensive GAEB format documentation
- Introduced detailed descriptions for GAEB format types: D-Format, X-Format, and P-Format.
- Included encoding specifications, structure, and record types for each format.
- Provided XML schema variations for X-Format with examples.
- Documented version history and parser implementation strategies.
- Highlighted common pitfalls and testing strategies for format detection and parsing.
- Outlined future enhancements for potential GAEB version support and performance optimizations.
</commit_message>
<xml_diff>
--- a/Data/Kalkulation_Abd.xlsx
+++ b/Data/Kalkulation_Abd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\absal\Dropbox\Ausschreibungen\Projekte_Vergabeportal\001.06_Maler_Bochum_15.07\04_Vergabeunterlagen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniduede-my.sharepoint.com/personal/mohamed_senhaby_stud_uni-due_de/Documents/PersonalWork/Laith/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2711240F-545A-47E5-95AC-CE67A9BD9ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{850D5F84-667B-4686-BBFD-73050A8BEC30}"/>
+    <workbookView xWindow="30450" yWindow="5700" windowWidth="21600" windowHeight="11295" xr2:uid="{850D5F84-667B-4686-BBFD-73050A8BEC30}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
   <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>